<commit_message>
fix bug and some optimize
</commit_message>
<xml_diff>
--- a/media/dtest/Untitled spreadsheet.xlsx
+++ b/media/dtest/Untitled spreadsheet.xlsx
@@ -273,17 +273,17 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,54 +586,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
-      <c r="F17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
-      <c r="F20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
-      <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>